<commit_message>
getRegister sorts keywords, checks input column wise
</commit_message>
<xml_diff>
--- a/tests/testthat/helper_register.xlsx
+++ b/tests/testthat/helper_register.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Benjamin_Becker\02_Repositories\packages\eatCodebook\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8947E593-1A5C-4930-A5B2-5102F23AECA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD54191-2ACB-4632-95C7-407EB2EB19A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8130" activeTab="1" xr2:uid="{D69379AA-37F0-4E49-B89B-0C726D28E0B1}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Nr.</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>some other label</t>
+  </si>
+  <si>
+    <t>keyword3</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B54C29-6551-4AFD-B94A-E7D7B904A0E1}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +495,7 @@
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,13 +506,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -526,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -537,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -546,6 +552,9 @@
       </c>
       <c r="C4" t="s">
         <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>